<commit_message>
Estableció colores en excel de salida
</commit_message>
<xml_diff>
--- a/ComparadorWebform/Archivos/Output/ArchivoComparacion_Galicia_27_01_2021.xlsx
+++ b/ComparadorWebform/Archivos/Output/ArchivoComparacion_Galicia_27_01_2021.xlsx
@@ -147,12 +147,27 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="5">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFA500"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF008000"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFFF00"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -174,16 +189,37 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -494,31 +530,31 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:5">
-      <x:c r="A1" s="0" t="s">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
-      <x:c r="A3" s="0" t="s">
+      <x:c r="A3" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
-      <x:c r="A4" s="0" t="s">
+      <x:c r="A4" s="3" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="B4" s="3" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="C4" s="3" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s">
+      <x:c r="D4" s="3" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
-      <x:c r="A5" s="1">
+      <x:c r="A5" s="4">
         <x:v>44200</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
@@ -529,7 +565,7 @@
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
-      <x:c r="A6" s="1">
+      <x:c r="A6" s="4">
         <x:v>44200</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
@@ -540,7 +576,7 @@
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
-      <x:c r="A7" s="1">
+      <x:c r="A7" s="4">
         <x:v>44200</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
@@ -551,7 +587,7 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
-      <x:c r="A8" s="1">
+      <x:c r="A8" s="4">
         <x:v>44200</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
@@ -562,7 +598,7 @@
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
-      <x:c r="A9" s="1">
+      <x:c r="A9" s="4">
         <x:v>44201</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
@@ -573,7 +609,7 @@
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
-      <x:c r="A10" s="1">
+      <x:c r="A10" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
@@ -584,7 +620,7 @@
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
-      <x:c r="A11" s="1">
+      <x:c r="A11" s="4">
         <x:v>44207</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
@@ -595,7 +631,7 @@
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
-      <x:c r="A12" s="1">
+      <x:c r="A12" s="4">
         <x:v>44215</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
@@ -606,7 +642,7 @@
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
-      <x:c r="A13" s="1">
+      <x:c r="A13" s="4">
         <x:v>44217</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
@@ -617,7 +653,7 @@
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
-      <x:c r="A14" s="1">
+      <x:c r="A14" s="4">
         <x:v>44218</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
@@ -628,12 +664,12 @@
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
-      <x:c r="A16" s="0" t="s">
+      <x:c r="A16" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
-      <x:c r="A17" s="0" t="s">
+      <x:c r="A17" s="3" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
@@ -647,7 +683,7 @@
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
-      <x:c r="A18" s="1">
+      <x:c r="A18" s="4">
         <x:v>44218</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
@@ -661,7 +697,7 @@
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
-      <x:c r="A19" s="1">
+      <x:c r="A19" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
@@ -675,7 +711,7 @@
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
-      <x:c r="A20" s="1">
+      <x:c r="A20" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
@@ -689,7 +725,7 @@
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
-      <x:c r="A21" s="1">
+      <x:c r="A21" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
@@ -703,7 +739,7 @@
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
-      <x:c r="A22" s="1">
+      <x:c r="A22" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
@@ -717,7 +753,7 @@
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
-      <x:c r="A23" s="1">
+      <x:c r="A23" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
@@ -731,7 +767,7 @@
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
-      <x:c r="A24" s="1">
+      <x:c r="A24" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
@@ -745,7 +781,7 @@
       </x:c>
     </x:row>
     <x:row r="25" spans="1:5">
-      <x:c r="A25" s="1">
+      <x:c r="A25" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
@@ -759,7 +795,7 @@
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
-      <x:c r="A26" s="1">
+      <x:c r="A26" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
@@ -773,7 +809,7 @@
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
-      <x:c r="A27" s="1">
+      <x:c r="A27" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
@@ -787,7 +823,7 @@
       </x:c>
     </x:row>
     <x:row r="28" spans="1:5">
-      <x:c r="A28" s="1">
+      <x:c r="A28" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
@@ -801,7 +837,7 @@
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
-      <x:c r="A29" s="1">
+      <x:c r="A29" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
@@ -815,7 +851,7 @@
       </x:c>
     </x:row>
     <x:row r="30" spans="1:5">
-      <x:c r="A30" s="1">
+      <x:c r="A30" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
@@ -829,7 +865,7 @@
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
-      <x:c r="A31" s="1">
+      <x:c r="A31" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
@@ -843,7 +879,7 @@
       </x:c>
     </x:row>
     <x:row r="32" spans="1:5">
-      <x:c r="A32" s="1">
+      <x:c r="A32" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
@@ -857,7 +893,7 @@
       </x:c>
     </x:row>
     <x:row r="33" spans="1:5">
-      <x:c r="A33" s="1">
+      <x:c r="A33" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
@@ -871,7 +907,7 @@
       </x:c>
     </x:row>
     <x:row r="34" spans="1:5">
-      <x:c r="A34" s="1">
+      <x:c r="A34" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
@@ -885,7 +921,7 @@
       </x:c>
     </x:row>
     <x:row r="35" spans="1:5">
-      <x:c r="A35" s="1">
+      <x:c r="A35" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
@@ -899,7 +935,7 @@
       </x:c>
     </x:row>
     <x:row r="36" spans="1:5">
-      <x:c r="A36" s="1">
+      <x:c r="A36" s="4">
         <x:v>44204</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
@@ -913,7 +949,7 @@
       </x:c>
     </x:row>
     <x:row r="38" spans="1:5">
-      <x:c r="A38" s="0" t="s">
+      <x:c r="A38" s="2" t="s">
         <x:v>32</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Se muestra en lo procesado que banco era
</commit_message>
<xml_diff>
--- a/ComparadorWebform/Archivos/Output/ArchivoComparacion_Galicia_27_01_2021.xlsx
+++ b/ComparadorWebform/Archivos/Output/ArchivoComparacion_Galicia_27_01_2021.xlsx
@@ -161,7 +161,7 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="FF008000"/>
+        <x:fgColor rgb="FF90EE90"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
@@ -672,13 +672,14 @@
       <x:c r="A17" s="3" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="C17" s="0" t="s">
+      <x:c r="B17" s="3" t="s"/>
+      <x:c r="C17" s="3" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
+      <x:c r="D17" s="3" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E17" s="0" t="s">
+      <x:c r="E17" s="3" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>

</xml_diff>